<commit_message>
data struct and extraction process completed
</commit_message>
<xml_diff>
--- a/dummy_data/ewts_master_dummy_data.xlsx
+++ b/dummy_data/ewts_master_dummy_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="EA_MD"/>
@@ -7688,7 +7688,7 @@
   </sheetPr>
   <dimension ref="A1:CF6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7703,10 +7703,10 @@
     <col min="9" max="9" style="20" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="20" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="19" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="19" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="19" width="37.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
@@ -8933,7 +8933,7 @@
   </sheetPr>
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8950,7 +8950,7 @@
     <col min="11" max="11" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="21" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="21" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="21" width="12.290714285714287" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="21" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="21" width="12.005" customWidth="1" bestFit="1"/>
@@ -8972,7 +8972,7 @@
     <col min="33" max="33" style="22" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="34" max="34" style="22" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="35" max="35" style="19" width="33.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="19" width="29.576428571428572" customWidth="1" bestFit="1"/>
     <col min="37" max="37" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="38" max="38" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="39" max="39" style="19" width="29.719285714285714" customWidth="1" bestFit="1"/>

</xml_diff>